<commit_message>
Made RestaurntScreen, incorporated it into the homescreen, made changes to the restaurantlist component
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -91,10 +91,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,12 +460,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -528,10 +528,18 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>43052</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="D6" s="2">
         <f t="shared" ref="D6:D35" si="0">ABS(C6-B6)</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,9 +719,9 @@
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>3.7500000000000013</v>
+        <v>4.5000000000000018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many changes, updated log
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -34,12 +34,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,10 +448,10 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -459,7 +459,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -467,7 +467,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -481,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>43052</v>
       </c>
@@ -497,7 +497,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>43052</v>
       </c>
@@ -512,7 +512,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
@@ -527,7 +527,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
@@ -542,186 +542,194 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>43053</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.3576388888888889</v>
+      </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.1666666666666685E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="5">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>4.5000000000000018</v>
+        <v>5.5000000000000018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on Restaurant Fetching, and displaying
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -34,12 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
-    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,12 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -447,11 +445,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -459,15 +457,15 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -481,14 +479,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43052</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.36458333333333331</v>
       </c>
       <c r="D3" s="2">
@@ -497,14 +495,14 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43052</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>0.38194444444444442</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.39583333333333331</v>
       </c>
       <c r="D4" s="2">
@@ -512,14 +510,14 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>0.72222222222222221</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>0.83333333333333337</v>
       </c>
       <c r="D5" s="2">
@@ -527,14 +525,14 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>0.92708333333333337</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>0.95833333333333337</v>
       </c>
       <c r="D6" s="2">
@@ -542,14 +540,14 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43053</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0.31597222222222221</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>0.3576388888888889</v>
       </c>
       <c r="D7" s="2">
@@ -557,179 +555,187 @@
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43053</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.92361111111111116</v>
+      </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:4">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:4">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:4">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:4">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:4">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:4">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:4">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:4">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:4">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:4">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:4">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:4">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:4">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:4">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:4">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:4">
-      <c r="D36" s="5">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>5.5000000000000018</v>
+        <v>8.5000000000000018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(UNTESTED) Changed order of tab and stack navigation, added stack navigation for search, started implementation of ListItem
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -34,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,7 +84,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -93,6 +93,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,11 +446,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -457,7 +458,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -465,7 +466,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -479,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>43052</v>
       </c>
@@ -495,7 +496,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>43052</v>
       </c>
@@ -510,7 +511,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
@@ -525,7 +526,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
@@ -540,7 +541,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>43053</v>
       </c>
@@ -555,7 +556,7 @@
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>43053</v>
       </c>
@@ -570,172 +571,181 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>43054</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.36458333333333331</v>
+      </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>8.5000000000000018</v>
+        <v>9.2500000000000018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited DIR Structure, code stucture, continued devolopment on listitem and restaurant list
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -90,10 +90,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -459,12 +459,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1">
       <c r="A2" t="s">
@@ -575,10 +575,10 @@
       <c r="A9" s="1">
         <v>43054</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.36458333333333331</v>
       </c>
       <c r="D9" s="2">
@@ -587,9 +587,18 @@
       </c>
     </row>
     <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>43054</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.4861111111111111</v>
+      </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.777777777777779E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -745,7 +754,7 @@
     <row r="36" spans="4:4">
       <c r="D36" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>9.2500000000000018</v>
+        <v>9.9166666666666679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to ListView and RestaurantList:
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -34,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,10 +447,10 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -458,7 +458,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -466,7 +466,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43052</v>
       </c>
@@ -496,7 +496,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43052</v>
       </c>
@@ -511,7 +511,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
@@ -526,7 +526,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
@@ -541,7 +541,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43053</v>
       </c>
@@ -556,7 +556,7 @@
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43053</v>
       </c>
@@ -571,7 +571,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43054</v>
       </c>
@@ -586,7 +586,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43054</v>
       </c>
@@ -601,7 +601,7 @@
         <v>2.777777777777779E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43054</v>
       </c>
@@ -616,7 +616,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43055</v>
       </c>
@@ -631,7 +631,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43055</v>
       </c>
@@ -646,7 +646,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43055</v>
       </c>
@@ -661,25 +661,37 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43055</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.76388888888888884</v>
+      </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+        <v>0.10416666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43055</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.86805555555555547</v>
+      </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>8.3333333333333259E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -688,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -697,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -706,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -715,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -724,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -733,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -742,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -751,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -760,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -769,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -778,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -787,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -796,7 +808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -805,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -814,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -823,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -832,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -841,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -850,10 +862,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>14.416666666666666</v>
+        <v>18.916666666666664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many changes: Added Rating, Logo, styling
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -34,11 +35,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,11 +447,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -458,7 +459,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -466,7 +467,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -480,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43052</v>
       </c>
@@ -496,7 +497,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43052</v>
       </c>
@@ -511,7 +512,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
@@ -526,7 +527,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
@@ -541,7 +542,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43053</v>
       </c>
@@ -556,7 +557,7 @@
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43053</v>
       </c>
@@ -571,7 +572,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43054</v>
       </c>
@@ -586,7 +587,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43054</v>
       </c>
@@ -601,7 +602,7 @@
         <v>2.777777777777779E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43054</v>
       </c>
@@ -616,7 +617,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43055</v>
       </c>
@@ -631,7 +632,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43055</v>
       </c>
@@ -646,7 +647,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43055</v>
       </c>
@@ -661,7 +662,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43055</v>
       </c>
@@ -676,7 +677,7 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43055</v>
       </c>
@@ -691,7 +692,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43056</v>
       </c>
@@ -706,7 +707,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43056</v>
       </c>
@@ -721,34 +722,52 @@
         <v>3.819444444444442E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43057</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.75347222222222221</v>
+      </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+        <v>2.430555555555558E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43057</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.84375</v>
+      </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+        <v>3.8194444444444531E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43057</v>
+      </c>
+      <c r="B21" s="2">
+        <v>43057.930555555555</v>
+      </c>
+      <c r="C21" s="2">
+        <v>43058.0625</v>
+      </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>0.13194444444525288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -757,7 +776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -766,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -775,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -784,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -793,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -802,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -811,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -820,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -829,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -838,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -847,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -856,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -865,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -874,10 +893,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>20.583333333333329</v>
+        <v>25.250000000019401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor chanages, added sidebar, and more listitem styling
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -447,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,12 +767,18 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="1">
+        <v>43058</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.291666666666663E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,7 +901,7 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>25.250000000019401</v>
+        <v>27.000000000019398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created About and Contact pages, worked on About page
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,12 +782,18 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="1">
+        <v>43058</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.92361111111111116</v>
+      </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -901,7 +907,7 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>27.000000000019398</v>
+        <v>29.000000000019401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Almost finished AboutScreen, added FAB to AboutScreen
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -34,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,7 +450,7 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -458,7 +458,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -466,7 +466,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43052</v>
       </c>
@@ -496,7 +496,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43052</v>
       </c>
@@ -511,7 +511,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
@@ -526,7 +526,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
@@ -541,7 +541,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43053</v>
       </c>
@@ -556,7 +556,7 @@
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43053</v>
       </c>
@@ -571,7 +571,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43054</v>
       </c>
@@ -586,7 +586,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43054</v>
       </c>
@@ -601,7 +601,7 @@
         <v>2.777777777777779E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43054</v>
       </c>
@@ -616,7 +616,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43055</v>
       </c>
@@ -631,7 +631,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43055</v>
       </c>
@@ -646,7 +646,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43055</v>
       </c>
@@ -661,7 +661,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43055</v>
       </c>
@@ -676,7 +676,7 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43055</v>
       </c>
@@ -691,7 +691,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43056</v>
       </c>
@@ -706,7 +706,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43056</v>
       </c>
@@ -721,7 +721,7 @@
         <v>3.819444444444442E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43057</v>
       </c>
@@ -736,7 +736,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43057</v>
       </c>
@@ -751,7 +751,7 @@
         <v>3.8194444444444531E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43057</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0.13194444444525288</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43058</v>
       </c>
@@ -781,7 +781,7 @@
         <v>7.291666666666663E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43058</v>
       </c>
@@ -796,7 +796,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43059</v>
       </c>
@@ -811,7 +811,7 @@
         <v>1.388888888888884E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43059</v>
       </c>
@@ -826,7 +826,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43059</v>
       </c>
@@ -841,16 +841,22 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43059</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>3.8194444444444531E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -859,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -868,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -877,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -886,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -895,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -904,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -913,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -922,10 +928,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>30.416666666686066</v>
+        <v>31.333333333352737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started working on Restaurant Screen, changed flow of HomeScreen, and MainContainer.
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,12 +857,18 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="1">
+        <v>43059</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.87847222222222221</v>
+      </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -931,7 +937,7 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>32.000000000019398</v>
+        <v>34.000000000019405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearranged HomeScreen, Worked on RestaurantScreen.
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -447,7 +447,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -857,30 +857,48 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="1">
+        <v>43060</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333259E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="1">
+        <v>43060</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.57291666666666663</v>
+      </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7777777777777679E-2</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="1">
+        <v>43060</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7777777777777679E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -931,7 +949,7 @@
     <row r="36" spans="1:4">
       <c r="D36" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>30.666666666686062</v>
+        <v>32.500000000019391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started Code Refactor to clean it up
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -34,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,7 +450,7 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -458,7 +458,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -466,7 +466,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>43052</v>
       </c>
@@ -496,7 +496,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>43052</v>
       </c>
@@ -511,7 +511,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
@@ -526,7 +526,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
@@ -541,7 +541,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>43053</v>
       </c>
@@ -556,7 +556,7 @@
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>43053</v>
       </c>
@@ -571,7 +571,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>43054</v>
       </c>
@@ -586,7 +586,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>43054</v>
       </c>
@@ -601,7 +601,7 @@
         <v>2.777777777777779E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>43054</v>
       </c>
@@ -616,7 +616,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>43055</v>
       </c>
@@ -631,7 +631,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>43055</v>
       </c>
@@ -646,7 +646,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>43055</v>
       </c>
@@ -661,7 +661,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>43055</v>
       </c>
@@ -676,7 +676,7 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>43055</v>
       </c>
@@ -691,7 +691,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>43056</v>
       </c>
@@ -706,7 +706,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>43056</v>
       </c>
@@ -721,7 +721,7 @@
         <v>3.819444444444442E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>43057</v>
       </c>
@@ -736,7 +736,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>43057</v>
       </c>
@@ -751,7 +751,7 @@
         <v>3.8194444444444531E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>43057</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0.13194444444525288</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>43058</v>
       </c>
@@ -781,7 +781,7 @@
         <v>7.291666666666663E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>43058</v>
       </c>
@@ -796,7 +796,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>43059</v>
       </c>
@@ -811,7 +811,7 @@
         <v>1.388888888888884E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>43059</v>
       </c>
@@ -826,7 +826,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>43059</v>
       </c>
@@ -841,7 +841,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>43060</v>
       </c>
@@ -856,7 +856,7 @@
         <v>1.041666666666663E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>43060</v>
       </c>
@@ -871,7 +871,7 @@
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>43060</v>
       </c>
@@ -886,7 +886,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>43060</v>
       </c>
@@ -901,7 +901,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>43061</v>
       </c>
@@ -916,7 +916,7 @@
         <v>2.0833333333333336E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>43062</v>
       </c>
@@ -931,7 +931,7 @@
         <v>5.5555555555555691E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>43064</v>
       </c>
@@ -946,7 +946,7 @@
         <v>4.861111111111116E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>43065</v>
       </c>
@@ -961,7 +961,7 @@
         <v>4.1666666666666671E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>43065</v>
       </c>
@@ -976,7 +976,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>43065</v>
       </c>
@@ -991,7 +991,7 @@
         <v>1.0416666666666685E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>43066</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>8.3333333333333343E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>43066</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>5.208333333333337E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>43067</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>0.11458333333333334</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>43068</v>
       </c>
@@ -1051,16 +1051,22 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>43069</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.3611111111111111</v>
+      </c>
       <c r="D41" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1069,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1078,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1087,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1096,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1105,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1114,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1123,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1132,10 +1138,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="D50" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>45.250000000019398</v>
+        <v>46.250000000019398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed RestaurantCard, and CardItem
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -34,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,10 +447,10 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -458,7 +458,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -466,7 +466,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43052</v>
       </c>
@@ -496,7 +496,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43052</v>
       </c>
@@ -511,7 +511,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
@@ -526,7 +526,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
@@ -541,7 +541,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43053</v>
       </c>
@@ -556,7 +556,7 @@
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43053</v>
       </c>
@@ -571,7 +571,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43054</v>
       </c>
@@ -586,7 +586,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43054</v>
       </c>
@@ -601,7 +601,7 @@
         <v>2.777777777777779E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43054</v>
       </c>
@@ -616,7 +616,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43055</v>
       </c>
@@ -631,7 +631,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43055</v>
       </c>
@@ -646,7 +646,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43055</v>
       </c>
@@ -661,7 +661,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43055</v>
       </c>
@@ -676,7 +676,7 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43055</v>
       </c>
@@ -691,7 +691,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43056</v>
       </c>
@@ -706,7 +706,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43056</v>
       </c>
@@ -721,7 +721,7 @@
         <v>3.819444444444442E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43057</v>
       </c>
@@ -736,7 +736,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43057</v>
       </c>
@@ -751,7 +751,7 @@
         <v>3.8194444444444531E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43057</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0.13194444444525288</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43058</v>
       </c>
@@ -781,7 +781,7 @@
         <v>7.291666666666663E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43058</v>
       </c>
@@ -796,7 +796,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43059</v>
       </c>
@@ -811,7 +811,7 @@
         <v>1.388888888888884E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43059</v>
       </c>
@@ -826,7 +826,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43059</v>
       </c>
@@ -841,7 +841,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43060</v>
       </c>
@@ -856,7 +856,7 @@
         <v>1.041666666666663E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43060</v>
       </c>
@@ -871,7 +871,7 @@
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43060</v>
       </c>
@@ -886,7 +886,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43060</v>
       </c>
@@ -901,7 +901,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43061</v>
       </c>
@@ -916,7 +916,7 @@
         <v>2.0833333333333336E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43062</v>
       </c>
@@ -931,7 +931,7 @@
         <v>5.5555555555555691E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43064</v>
       </c>
@@ -950,7 +950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43065</v>
       </c>
@@ -965,7 +965,7 @@
         <v>4.1666666666666671E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43065</v>
       </c>
@@ -980,7 +980,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43065</v>
       </c>
@@ -995,7 +995,7 @@
         <v>1.0416666666666685E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43066</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>8.3333333333333343E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43066</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>5.208333333333337E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43067</v>
       </c>
@@ -1040,22 +1040,22 @@
         <v>0.11458333333333334</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43068</v>
       </c>
       <c r="B40" s="2">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="C40" s="2">
-        <v>0.3125</v>
+        <v>0.8125</v>
       </c>
       <c r="D40" s="2">
         <f t="shared" ref="D40:D49" si="2">ABS(C40-B40)</f>
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43069</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43069</v>
       </c>
@@ -1085,16 +1085,22 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43069</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.76388888888888884</v>
+      </c>
       <c r="D43" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>5.5555555555555469E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1103,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1112,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1121,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1130,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1139,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1148,10 +1154,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>47.000000000019398</v>
+        <v>48.333333333352726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integrated expo, fixing icons
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -1101,12 +1101,16 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="2"/>
+      <c r="A44" s="1">
+        <v>43071</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1157,7 +1161,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>48.333333333352726</v>
+        <v>70.333333333352726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated logs, fixing icons
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -1105,12 +1105,14 @@
         <v>43071</v>
       </c>
       <c r="B44" s="2">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="C44" s="2"/>
+        <v>43071.916666666664</v>
+      </c>
+      <c r="C44" s="2">
+        <v>43072</v>
+      </c>
       <c r="D44" s="2">
         <f t="shared" si="2"/>
-        <v>0.91666666666666663</v>
+        <v>8.3333333335758653E-2</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1161,7 +1163,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>70.333333333352726</v>
+        <v>50.333333333410934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got everything working and converted
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +931,7 @@
         <v>5.5555555555555691E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43064</v>
       </c>
@@ -945,12 +945,8 @@
         <f t="shared" si="0"/>
         <v>4.861111111111116E-2</v>
       </c>
-      <c r="G33">
-        <f>30-13</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43065</v>
       </c>
@@ -965,7 +961,7 @@
         <v>4.1666666666666671E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43065</v>
       </c>
@@ -980,7 +976,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43065</v>
       </c>
@@ -995,7 +991,7 @@
         <v>1.0416666666666685E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43066</v>
       </c>
@@ -1010,7 +1006,7 @@
         <v>8.3333333333333343E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43066</v>
       </c>
@@ -1025,7 +1021,7 @@
         <v>5.208333333333337E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43067</v>
       </c>
@@ -1040,7 +1036,7 @@
         <v>0.11458333333333334</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43068</v>
       </c>
@@ -1055,7 +1051,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43069</v>
       </c>
@@ -1070,7 +1066,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43069</v>
       </c>
@@ -1085,7 +1081,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43069</v>
       </c>
@@ -1100,7 +1096,7 @@
         <v>5.5555555555555469E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43071</v>
       </c>
@@ -1115,25 +1111,37 @@
         <v>8.3333333335758653E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43072</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="D45" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+        <v>0.13541666666666674</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43072</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="D46" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2.0833333333333259E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1142,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1163,7 +1171,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>50.333333333410934</v>
+        <v>54.083333333410927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Patched RestaurantList and SideBar
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,12 +1142,16 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2"/>
+      <c r="A47" s="1">
+        <v>43079</v>
+      </c>
+      <c r="B47" s="2">
+        <v>6.9444444444444434E-2</v>
+      </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.9444444444444434E-2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,7 +1175,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>54.083333333410927</v>
+        <v>55.750000000077598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started implementing restaurant card refactor
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -447,7 +447,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,10 +1148,12 @@
       <c r="B47" s="2">
         <v>6.9444444444444434E-2</v>
       </c>
-      <c r="C47" s="2"/>
+      <c r="C47" s="2">
+        <v>8.6805555555555566E-2</v>
+      </c>
       <c r="D47" s="2">
         <f t="shared" si="2"/>
-        <v>6.9444444444444434E-2</v>
+        <v>1.7361111111111133E-2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,7 +1177,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>55.750000000077598</v>
+        <v>54.500000000077591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on Styling Refactor
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -34,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,10 +447,10 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -458,7 +458,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -466,7 +466,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>43052</v>
       </c>
@@ -496,7 +496,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>43052</v>
       </c>
@@ -511,7 +511,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
@@ -526,7 +526,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
@@ -541,7 +541,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>43053</v>
       </c>
@@ -556,7 +556,7 @@
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>43053</v>
       </c>
@@ -571,7 +571,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>43054</v>
       </c>
@@ -586,7 +586,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>43054</v>
       </c>
@@ -601,7 +601,7 @@
         <v>2.777777777777779E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>43054</v>
       </c>
@@ -616,7 +616,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>43055</v>
       </c>
@@ -631,7 +631,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>43055</v>
       </c>
@@ -646,7 +646,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>43055</v>
       </c>
@@ -661,7 +661,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>43055</v>
       </c>
@@ -676,7 +676,7 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>43055</v>
       </c>
@@ -691,7 +691,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>43056</v>
       </c>
@@ -706,7 +706,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>43056</v>
       </c>
@@ -721,7 +721,7 @@
         <v>3.819444444444442E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>43057</v>
       </c>
@@ -736,7 +736,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>43057</v>
       </c>
@@ -751,7 +751,7 @@
         <v>3.8194444444444531E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>43057</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0.13194444444525288</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>43058</v>
       </c>
@@ -781,7 +781,7 @@
         <v>7.291666666666663E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>43058</v>
       </c>
@@ -796,7 +796,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>43059</v>
       </c>
@@ -811,7 +811,7 @@
         <v>1.388888888888884E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>43059</v>
       </c>
@@ -826,7 +826,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>43059</v>
       </c>
@@ -841,7 +841,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>43060</v>
       </c>
@@ -856,7 +856,7 @@
         <v>1.041666666666663E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>43060</v>
       </c>
@@ -871,7 +871,7 @@
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>43060</v>
       </c>
@@ -886,7 +886,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>43060</v>
       </c>
@@ -901,7 +901,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>43061</v>
       </c>
@@ -916,7 +916,7 @@
         <v>2.0833333333333336E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>43062</v>
       </c>
@@ -931,7 +931,7 @@
         <v>5.5555555555555691E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>43064</v>
       </c>
@@ -946,7 +946,7 @@
         <v>4.861111111111116E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>43065</v>
       </c>
@@ -961,7 +961,7 @@
         <v>4.1666666666666671E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>43065</v>
       </c>
@@ -976,7 +976,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>43065</v>
       </c>
@@ -991,7 +991,7 @@
         <v>1.0416666666666685E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>43066</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>8.3333333333333343E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>43066</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>5.208333333333337E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>43067</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>0.11458333333333334</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>43068</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>43069</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>43069</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>43069</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>5.5555555555555469E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>43071</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>8.3333333335758653E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>43072</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>0.13541666666666674</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>43072</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>43079</v>
       </c>
@@ -1156,16 +1156,22 @@
         <v>1.7361111111111133E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>43080</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.48958333333333331</v>
+      </c>
       <c r="D48" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1174,10 +1180,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="D50" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>54.500000000077591</v>
+        <v>55.250000000077591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished RestaurantCard Refactor #2
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -34,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,8 +143,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D50" totalsRowCount="1">
-  <autoFilter ref="A2:D49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D59" totalsRowCount="1">
+  <autoFilter ref="A2:D58"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Date"/>
     <tableColumn id="2" name="Start Time"/>
@@ -444,13 +444,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -458,7 +458,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -466,7 +466,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43052</v>
       </c>
@@ -496,7 +496,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43052</v>
       </c>
@@ -511,7 +511,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
@@ -526,7 +526,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
@@ -541,7 +541,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43053</v>
       </c>
@@ -556,7 +556,7 @@
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43053</v>
       </c>
@@ -571,7 +571,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43054</v>
       </c>
@@ -586,7 +586,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43054</v>
       </c>
@@ -601,7 +601,7 @@
         <v>2.777777777777779E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43054</v>
       </c>
@@ -616,7 +616,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43055</v>
       </c>
@@ -631,7 +631,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43055</v>
       </c>
@@ -646,7 +646,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43055</v>
       </c>
@@ -661,7 +661,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43055</v>
       </c>
@@ -676,7 +676,7 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43055</v>
       </c>
@@ -691,7 +691,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43056</v>
       </c>
@@ -706,7 +706,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43056</v>
       </c>
@@ -721,7 +721,7 @@
         <v>3.819444444444442E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43057</v>
       </c>
@@ -736,7 +736,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43057</v>
       </c>
@@ -751,7 +751,7 @@
         <v>3.8194444444444531E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43057</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0.13194444444525288</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43058</v>
       </c>
@@ -781,7 +781,7 @@
         <v>7.291666666666663E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43058</v>
       </c>
@@ -796,7 +796,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43059</v>
       </c>
@@ -811,7 +811,7 @@
         <v>1.388888888888884E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43059</v>
       </c>
@@ -826,7 +826,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43059</v>
       </c>
@@ -841,7 +841,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43060</v>
       </c>
@@ -856,7 +856,7 @@
         <v>1.041666666666663E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43060</v>
       </c>
@@ -871,7 +871,7 @@
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43060</v>
       </c>
@@ -886,7 +886,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43060</v>
       </c>
@@ -901,7 +901,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43061</v>
       </c>
@@ -916,7 +916,7 @@
         <v>2.0833333333333336E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43062</v>
       </c>
@@ -931,7 +931,7 @@
         <v>5.5555555555555691E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43064</v>
       </c>
@@ -946,7 +946,7 @@
         <v>4.861111111111116E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43065</v>
       </c>
@@ -961,7 +961,7 @@
         <v>4.1666666666666671E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43065</v>
       </c>
@@ -976,7 +976,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43065</v>
       </c>
@@ -991,7 +991,7 @@
         <v>1.0416666666666685E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43066</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>8.3333333333333343E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43066</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>5.208333333333337E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43067</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>0.11458333333333334</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43068</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43069</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43069</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43069</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>5.5555555555555469E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43071</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>8.3333333335758653E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43072</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>0.13541666666666674</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43072</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43079</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>1.7361111111111133E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43080</v>
       </c>
@@ -1171,19 +1171,110 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43080</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.75</v>
+      </c>
       <c r="D49" s="2">
         <f t="shared" si="2"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43080</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2">
+        <f t="shared" ref="D50:D58" si="3">ABS(C50-B50)</f>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="D50" s="4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="4">
         <f>SUM(Table1[Work Time])*24</f>
-        <v>55.250000000077591</v>
+        <v>77.250000000077591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>